<commit_message>
Refactored Data Model for Decision Support for improved readability and maintainability
</commit_message>
<xml_diff>
--- a/LEARNING & PROGRESS TRACKER.xlsx
+++ b/LEARNING & PROGRESS TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8ca8857e943fa77/Documents/FORMAL CURRICULUM PROGRAMME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8ca8857e943fa77/Documents/FORMAL CURRICULUM PROGRAMME/Decision-Driven Analytics Curriculum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{3F893D99-B140-4980-89A3-A1297C14FB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F836EBB7-4839-417E-9B30-84711C012A77}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{3F893D99-B140-4980-89A3-A1297C14FB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD785C69-2E69-4643-B1BD-8BC7A27C0CE1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1AA1A007-8949-49C8-A2C3-ADCB6D477152}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Module</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>94/100</t>
+  </si>
+  <si>
+    <t>07/01/2026</t>
+  </si>
+  <si>
+    <t>92/100</t>
+  </si>
+  <si>
+    <t>Add a short “Model Scope &amp; Assumptions” section
+Acknowledge implied dimensions
+Clarify drawdown and risk calculation assumptions
+Slightly strengthen the Design Justification language</t>
   </si>
 </sst>
 </file>
@@ -596,11 +608,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227F1576-FAB1-4893-A07F-EA33009C4D65}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -680,25 +695,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
Added Hypothesis-Driven Exploratory Analysis module breakdown document
</commit_message>
<xml_diff>
--- a/LEARNING & PROGRESS TRACKER.xlsx
+++ b/LEARNING & PROGRESS TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8ca8857e943fa77/Documents/FORMAL CURRICULUM PROGRAMME/Decision-Driven Analytics Curriculum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\FORMAL CURRICULUM PROGRAMME\Decision-Driven Analytics Self-Paced Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{3F893D99-B140-4980-89A3-A1297C14FB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD785C69-2E69-4643-B1BD-8BC7A27C0CE1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DAAD6D-1C11-4EB4-9E0B-E1AE325CEC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{1AA1A007-8949-49C8-A2C3-ADCB6D477152}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="39">
   <si>
     <t>Module</t>
   </si>
@@ -156,6 +156,9 @@
 Acknowledge implied dimensions
 Clarify drawdown and risk calculation assumptions
 Slightly strengthen the Design Justification language</t>
+  </si>
+  <si>
+    <t>08/01/2025</t>
   </si>
 </sst>
 </file>
@@ -608,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227F1576-FAB1-4893-A07F-EA33009C4D65}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +672,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -695,7 +698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -725,10 +728,12 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
         <v>8</v>

</xml_diff>